<commit_message>
struggling with keyword driven frameworkgit status !
</commit_message>
<xml_diff>
--- a/com.demoqa/ExcelFiles/DemoQATest.xlsx
+++ b/com.demoqa/ExcelFiles/DemoQATest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6150" windowWidth="28860" windowHeight="6210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10035" windowHeight="3960"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:C11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>Path</t>
   </si>
@@ -63,9 +64,6 @@
     <t>Steps</t>
   </si>
   <si>
-    <t>Action</t>
-  </si>
-  <si>
     <t>locator Type</t>
   </si>
   <si>
@@ -181,13 +179,88 @@
   </si>
   <si>
     <t>submit</t>
+  </si>
+  <si>
+    <t>User Action</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>alexander@hamilton.com</t>
+  </si>
+  <si>
+    <t>123-412-1234</t>
+  </si>
+  <si>
+    <t>just a Subject</t>
+  </si>
+  <si>
+    <t>321 Baker st</t>
+  </si>
+  <si>
+    <t>Step 2</t>
+  </si>
+  <si>
+    <t>Step 3</t>
+  </si>
+  <si>
+    <t>Step 4</t>
+  </si>
+  <si>
+    <t>Step 5</t>
+  </si>
+  <si>
+    <t>Step 6</t>
+  </si>
+  <si>
+    <t>Step 7</t>
+  </si>
+  <si>
+    <t>Step 8</t>
+  </si>
+  <si>
+    <t>Step 9</t>
+  </si>
+  <si>
+    <t>Step 10</t>
+  </si>
+  <si>
+    <t>Step 11</t>
+  </si>
+  <si>
+    <t>Step 12</t>
+  </si>
+  <si>
+    <t>Step 13</t>
+  </si>
+  <si>
+    <t>Step 14</t>
+  </si>
+  <si>
+    <t>Step 15</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>fileLocation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +275,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -227,15 +307,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -530,7 +617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -595,24 +682,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -626,235 +714,328 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
         <v>37</v>
       </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="4">
+        <v>30379</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
         <v>37</v>
       </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" t="s">
-        <v>54</v>
+      <c r="H16" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
struggling with keyword driven framework, looks easy but needs lot of mind work !
</commit_message>
<xml_diff>
--- a/com.demoqa/ExcelFiles/DemoQATest.xlsx
+++ b/com.demoqa/ExcelFiles/DemoQATest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="10035" windowHeight="3960"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="7125" windowHeight="3960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:C11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>Path</t>
   </si>
@@ -245,12 +244,6 @@
   </si>
   <si>
     <t>Data</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>url</t>
   </si>
   <si>
     <t>fileLocation</t>
@@ -617,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -684,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -749,7 +742,7 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -769,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -949,7 +942,7 @@
         <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8">

</xml_diff>

<commit_message>
Finally got keyword driven framework to work witha few hickups git push git push
</commit_message>
<xml_diff>
--- a/com.demoqa/ExcelFiles/DemoQATest.xlsx
+++ b/com.demoqa/ExcelFiles/DemoQATest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Path</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Enter Phone number</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter Date </t>
-  </si>
-  <si>
     <t xml:space="preserve">Enter Subject </t>
   </si>
   <si>
@@ -156,12 +153,6 @@
     <t>mobileNumber</t>
   </si>
   <si>
-    <t>dateOfBirth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subjects </t>
-  </si>
-  <si>
     <t>hobbiesSport</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>Step 7</t>
   </si>
   <si>
-    <t>Step 8</t>
-  </si>
-  <si>
     <t>Step 9</t>
   </si>
   <si>
@@ -247,6 +235,27 @@
   </si>
   <si>
     <t>fileLocation</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>Blose browser</t>
+  </si>
+  <si>
+    <t>Close Browser</t>
+  </si>
+  <si>
+    <t>NCR</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>subjects</t>
   </si>
 </sst>
 </file>
@@ -307,12 +316,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -677,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -707,7 +715,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>15</v>
@@ -716,7 +724,7 @@
         <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -742,18 +750,18 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="C3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -762,152 +770,152 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="C4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="C6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="C7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="C8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="C9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="4">
-        <v>30379</v>
+        <v>79</v>
+      </c>
+      <c r="H9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="C10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="C11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -916,38 +924,38 @@
         <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="C12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="C13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -956,70 +964,67 @@
         <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="C14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14">
-        <v>4</v>
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="C15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="C16" t="s">
-        <v>74</v>
-      </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
         <v>20</v>

</xml_diff>